<commit_message>
Ajustements esthétiques dans les modèles
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_adherents.xlsx
+++ b/fichiers/conf/modele_adherents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65A35D1-B51E-4902-83C4-76255184AE18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C32DDB-DA7D-4A3B-9950-A12E1B03FC16}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="472" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="1530" yWindow="495" windowWidth="22905" windowHeight="13815" tabRatio="472" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adhérents" sheetId="1" r:id="rId1"/>
@@ -694,7 +694,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +709,7 @@
     <col min="8" max="9" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Registre de présence et simplification des interfaces
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_adherents.xlsx
+++ b/fichiers/conf/modele_adherents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D289B40-CCEB-417A-ADF8-0FE666E08C27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734C77D5-1DA1-42EA-854B-DB08814F92CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="439" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="439" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adhérents" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Aide" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Adhérents!$A$1:$K$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Adhérents!$A$1:$M$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Effectifs!$A$1:$D$2</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -155,6 +155,18 @@
   </si>
   <si>
     <t>${adherent.brancheanneeprochaine}</t>
+  </si>
+  <si>
+    <t>Date de naissance</t>
+  </si>
+  <si>
+    <t>${adherent.datedenaissance}</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>${adherent.age}</t>
   </si>
 </sst>
 </file>
@@ -688,11 +700,11 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,16 +712,17 @@
     <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" customWidth="1"/>
     <col min="3" max="3" width="37.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="57.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9" style="2" customWidth="1"/>
-    <col min="10" max="11" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="57.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9" style="2" customWidth="1"/>
+    <col min="12" max="13" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -720,31 +733,37 @@
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -754,37 +773,43 @@
       <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K2" xr:uid="{50C0CF3F-2DAB-4597-855F-3644F39C68A4}"/>
-  <conditionalFormatting sqref="H2:H1048576">
+  <autoFilter ref="A1:M2" xr:uid="{50C0CF3F-2DAB-4597-855F-3644F39C68A4}"/>
+  <conditionalFormatting sqref="J2:J1048576">
     <cfRule type="cellIs" dxfId="7" priority="37" stopIfTrue="1" operator="between">
       <formula>240</formula>
       <formula>240</formula>
@@ -810,12 +835,12 @@
       <formula>219</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J1048576">
+  <conditionalFormatting sqref="L2:L1048576">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K1048576">
+  <conditionalFormatting sqref="M2:M1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
@@ -832,7 +857,7 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A4:XFD5"/>
     </sheetView>

</xml_diff>

<commit_message>
Gestion du droit à l'image pour les adhérents
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_adherents.xlsx
+++ b/fichiers/conf/modele_adherents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734C77D5-1DA1-42EA-854B-DB08814F92CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CAF8BE-0F31-4045-B962-8D1A9BA3A131}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="439" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="391" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adhérents" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Aide" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Adhérents!$A$1:$M$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Adhérents!$A$1:$N$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Effectifs!$A$1:$D$2</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>${adherent.age}</t>
+  </si>
+  <si>
+    <t>Droit à l'image OK ?</t>
+  </si>
+  <si>
+    <t>${adherent.droitimageok}</t>
   </si>
 </sst>
 </file>
@@ -301,7 +307,107 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF007E39"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -700,7 +806,7 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -720,9 +826,11 @@
     <col min="10" max="10" width="15.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="9" style="2" customWidth="1"/>
     <col min="12" max="13" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -762,8 +870,11 @@
       <c r="M1" s="12" t="s">
         <v>31</v>
       </c>
+      <c r="N1" s="12" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -803,45 +914,53 @@
       <c r="M2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M2" xr:uid="{50C0CF3F-2DAB-4597-855F-3644F39C68A4}"/>
+  <autoFilter ref="A1:N2" xr:uid="{1F72967C-D7F3-41E2-9BA2-82E68CFB32EC}"/>
   <conditionalFormatting sqref="J2:J1048576">
-    <cfRule type="cellIs" dxfId="7" priority="37" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="38" stopIfTrue="1" operator="between">
       <formula>240</formula>
       <formula>240</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="38" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="39" stopIfTrue="1" operator="between">
       <formula>270</formula>
       <formula>271</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="39" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="40" stopIfTrue="1" operator="between">
       <formula>300</formula>
       <formula>999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="40" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="41" stopIfTrue="1" operator="between">
       <formula>230</formula>
       <formula>239</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="41" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="42" stopIfTrue="1" operator="between">
       <formula>220</formula>
       <formula>229</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="42" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="43" stopIfTrue="1" operator="between">
       <formula>210</formula>
       <formula>219</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N1048576">
+    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -859,7 +978,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A4:XFD5"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Rajout des code groupe et structure
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_adherents.xlsx
+++ b/fichiers/conf/modele_adherents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CAF8BE-0F31-4045-B962-8D1A9BA3A131}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A657359-CD99-4EC6-817D-B134C132C137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="391" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="1650" yWindow="1440" windowWidth="27150" windowHeight="14160" tabRatio="391" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adhérents" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Aide" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Adhérents!$A$1:$N$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Adhérents!$A$1:$P$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Effectifs!$A$1:$D$2</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -173,6 +173,18 @@
   </si>
   <si>
     <t>${adherent.droitimageok}</t>
+  </si>
+  <si>
+    <t>Code Groupe</t>
+  </si>
+  <si>
+    <t>Code Structure</t>
+  </si>
+  <si>
+    <t>${adherent.codegroupe}</t>
+  </si>
+  <si>
+    <t>${adherent.codestructure}</t>
   </si>
 </sst>
 </file>
@@ -257,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -303,101 +315,17 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF007E39"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -806,7 +734,7 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -821,16 +749,18 @@
     <col min="4" max="4" width="29.42578125" style="2" customWidth="1"/>
     <col min="5" max="6" width="12.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="57.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9" style="2" customWidth="1"/>
-    <col min="12" max="13" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="9" style="2" customWidth="1"/>
+    <col min="14" max="15" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -852,29 +782,35 @@
       <c r="G1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -896,71 +832,77 @@
       <c r="G2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="K2" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N2" xr:uid="{1F72967C-D7F3-41E2-9BA2-82E68CFB32EC}"/>
-  <conditionalFormatting sqref="J2:J1048576">
-    <cfRule type="cellIs" dxfId="17" priority="38" stopIfTrue="1" operator="between">
+  <autoFilter ref="A1:P2" xr:uid="{1F72967C-D7F3-41E2-9BA2-82E68CFB32EC}"/>
+  <conditionalFormatting sqref="L2:L1048576">
+    <cfRule type="cellIs" dxfId="8" priority="38" stopIfTrue="1" operator="between">
       <formula>240</formula>
       <formula>240</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="39" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="39" stopIfTrue="1" operator="between">
       <formula>270</formula>
       <formula>271</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="40" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="40" stopIfTrue="1" operator="between">
       <formula>300</formula>
       <formula>999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="41" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="41" stopIfTrue="1" operator="between">
       <formula>230</formula>
       <formula>239</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="42" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="42" stopIfTrue="1" operator="between">
       <formula>220</formula>
       <formula>229</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="43" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="43" stopIfTrue="1" operator="between">
       <formula>210</formula>
       <formula>219</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L1048576">
-    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="N2:N1048576">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M1048576">
-    <cfRule type="cellIs" dxfId="10" priority="2" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="O2:O1048576">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="P2:P1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Squelette poor la gestion des alertes
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_adherents.xlsx
+++ b/fichiers/conf/modele_adherents.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A657359-CD99-4EC6-817D-B134C132C137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8611E330-F5FD-46FD-93F2-3F5F1836B03C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="1440" windowWidth="27150" windowHeight="14160" tabRatio="391" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="1395" yWindow="840" windowWidth="27150" windowHeight="14160" tabRatio="391" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adhérents" sheetId="1" r:id="rId1"/>
     <sheet name="Effectifs" sheetId="2" r:id="rId2"/>
-    <sheet name="Global" sheetId="5" r:id="rId3"/>
-    <sheet name="Général" sheetId="6" r:id="rId4"/>
-    <sheet name="Aide" sheetId="4" r:id="rId5"/>
+    <sheet name="Alertes" sheetId="7" r:id="rId3"/>
+    <sheet name="Global" sheetId="5" r:id="rId4"/>
+    <sheet name="Général" sheetId="6" r:id="rId5"/>
+    <sheet name="Aide" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Adhérents!$A$1:$P$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Effectifs!$A$1:$D$2</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,6 +32,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -185,6 +189,42 @@
   </si>
   <si>
     <t>${adherent.codestructure}</t>
+  </si>
+  <si>
+    <t>Sévérité</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Erreur</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${alertes}" var="alerte" orderBy="severite;type"&gt;${alerte.adherent.code}</t>
+  </si>
+  <si>
+    <t>${alerte.adherent.unite}</t>
+  </si>
+  <si>
+    <t>${alerte.adherent.codegroupe}</t>
+  </si>
+  <si>
+    <t>${alerte.adherent.codestructure}</t>
+  </si>
+  <si>
+    <t>${alerte.adherent.nom}</t>
+  </si>
+  <si>
+    <t>${alerte.adherent.prenom}</t>
+  </si>
+  <si>
+    <t>${alerte.severite}</t>
+  </si>
+  <si>
+    <t>${alerte.type}</t>
+  </si>
+  <si>
+    <t>${alerte.message}</t>
   </si>
 </sst>
 </file>
@@ -760,7 +800,7 @@
     <col min="17" max="17" width="18.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -973,6 +1013,96 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7174CF0-DD7B-434D-8E9C-34A2F79E3C5F}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="57.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" customWidth="1"/>
+    <col min="6" max="6" width="37.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" customWidth="1"/>
+    <col min="9" max="9" width="86.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC5C4104-3EAE-4F48-A5B4-34DC074AB0B8}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1005,7 +1135,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831EBE71-927E-45DB-B6B5-3EB816C571F7}">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -1049,7 +1179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FF42C4-E612-4A2B-8582-F0FFD086172F}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>

</xml_diff>